<commit_message>
debug train ann and generate new report
</commit_message>
<xml_diff>
--- a/data/optimization_results.xlsx
+++ b/data/optimization_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9981.625679984112</v>
+        <v>9950.553538281036</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>462.470649717059</v>
+        <v>507.8029377984964</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8944.504220828099</v>
+        <v>9705.990876641363</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>CSTR1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -509,13 +509,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4000</v>
+        <v>3687.452875457066</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>CSTR1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -524,172 +524,52 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>460.4583777822451</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>C1_surface_area</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KLa</t>
+          <t>C1_height</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>421.6160198117984</v>
+        <v>5.107451673317976</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>O1</t>
+          <t>CSTR1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CSTR1_split_internal</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3513.984522373709</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>O1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>KLa</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>455.7833425069027</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>O2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>O2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>KLa</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>429.6731768325639</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>O3</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>3687.452875457066</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>O3</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>KLa</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>460.4583777822451</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>C1_surface_area</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>C1_height</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>6.01191402680718</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>O3</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>O3_split_internal</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.3270748212356701</v>
+        <v>0.1997683856365939</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +864,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,47 +887,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOD_A1</t>
+          <t>BOD_CSTR1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>607.265214337428</v>
+        <v>611.6814262544357</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>COD_A1</t>
+          <t>COD_CSTR1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6731.511399869436</v>
+        <v>6799.011337400194</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TKN_A1</t>
+          <t>TKN_CSTR1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>208.42783908035</v>
+        <v>219.5986281802594</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TN_A1</t>
+          <t>TN_CSTR1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>295.8378432015441</v>
+        <v>302.052027684968</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TP_A1</t>
+          <t>TP_CSTR1</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1057,651 +937,251 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TSS_A1</t>
+          <t>TSS_CSTR1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5917.262147825887</v>
+        <v>4946.454791319757</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VSS_A1</t>
+          <t>VSS_CSTR1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4898.246857605723</v>
+        <v>4431.120631762057</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>X_AUT_A1</t>
+          <t>X_AUT_CSTR1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>60.3273602907266</v>
+        <v>62.22426883969838</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>X_H_A1</t>
+          <t>X_H_CSTR1</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>740.6919948679367</v>
+        <v>884.382387479484</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>X_PAO_A1</t>
+          <t>X_PAO_CSTR1</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46.20916610716439</v>
+        <v>38.35500170632851</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BOD_A2</t>
+          <t>BOD_Effluent</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>589.0053169068656</v>
+        <v>34.35575593759587</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>COD_A2</t>
+          <t>BOD_Wastage</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7024.509074669612</v>
+        <v>1141.695823041204</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TKN_A2</t>
+          <t>COD_Effluent</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>213.2732902092059</v>
+        <v>679.2187760828191</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TN_A2</t>
+          <t>COD_Wastage</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>303.962645514275</v>
+        <v>12890.33334015606</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TP_A2</t>
+          <t>TKN_Effluent</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>301.410659170956</v>
+        <v>33.25353424018757</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TSS_A2</t>
+          <t>TKN_Wastage</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4946.454791319757</v>
+        <v>393.8412470978733</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>VSS_A2</t>
+          <t>TN_Effluent</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4801.899290309422</v>
+        <v>157.6179015388149</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>X_AUT_A2</t>
+          <t>TN_Wastage</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>66.83164503716164</v>
+        <v>532.4126125993653</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>X_H_A2</t>
+          <t>TP_Effluent</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>835.7166546854567</v>
+        <v>166.2676711344307</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>X_PAO_A2</t>
+          <t>TP_Wastage</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>42.54580835492751</v>
+        <v>435.3389328960134</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BOD_O1</t>
+          <t>TSS_Effluent</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>574.2341068625669</v>
+        <v>262.5190725169087</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>COD_O1</t>
+          <t>TSS_Wastage</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>7084.607346499512</v>
+        <v>11129.63417806069</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TKN_O1</t>
+          <t>VSS_Effluent</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>209.1045957988432</v>
+        <v>231.264168426842</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TN_O1</t>
+          <t>VSS_Wastage</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>295.8378432015441</v>
+        <v>9490.984727580864</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TP_O1</t>
+          <t>X_AUT_Effluent</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>290.3098652538909</v>
+        <v>4.126452430775707</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TSS_O1</t>
+          <t>X_AUT_Wastage</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5018.514593746215</v>
+        <v>120.6792640639327</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>VSS_O1</t>
+          <t>X_H_Effluent</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4946.454791319758</v>
+        <v>42.53368853028554</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>X_AUT_O1</t>
+          <t>X_H_Wastage</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>62.70281830017213</v>
+        <v>1894.019400391027</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>X_H_O1</t>
+          <t>X_PAO_Effluent</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>740.6919948679371</v>
+        <v>1.854052159803666</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>X_PAO_O1</t>
+          <t>X_PAO_Wastage</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>41.79184537105311</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>BOD_O2</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>607.6013727739971</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>COD_O2</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>6692.694924610366</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>TKN_O2</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>217.9980525548408</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>TN_O2</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>295.8378432015441</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>TP_O2</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>294.1929185923519</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>TSS_O2</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>4946.454791319766</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>VSS_O2</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>4659.596839528162</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>X_AUT_O2</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>50.27758713229958</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>X_H_O2</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>740.6919948679367</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>X_PAO_O2</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>45.38455881536931</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>BOD_O3</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>638.302376713069</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>COD_O3</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>8009.67552799563</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>TKN_O3</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>221.8583735353482</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>TN_O3</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>323.648628513309</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>TP_O3</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>306.9835118461574</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>TSS_O3</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>4946.454791319757</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>VSS_O3</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>4946.454791319784</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>X_AUT_O3</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>69.04319744715279</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>X_H_O3</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>789.5667982073164</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>X_PAO_O3</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>50.27758713229959</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>BOD_Effluent</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>30.28014014042899</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>BOD_Wastage</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>1061.288784583341</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>COD_Effluent</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>673.139019756272</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>COD_Wastage</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>13193.69723964875</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>TKN_Effluent</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>30.95485279414541</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>TKN_Wastage</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>386.102960640127</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>TN_Effluent</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>151.1830456348136</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>TN_Wastage</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>521.7652904644993</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>TP_Effluent</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>166.2676711344307</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>TP_Wastage</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>440.9951535542905</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>TSS_Effluent</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>264.2862802638527</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>TSS_Wastage</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>11174.43788457828</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>VSS_Effluent</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>295.8378432015435</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>VSS_Wastage</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>9589.54526217734</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>X_AUT_Effluent</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>2.992437396175996</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>X_AUT_Wastage</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>119.1646162768412</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>X_H_Effluent</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>37.77594757766878</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>X_H_Wastage</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>1583.386087511009</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>X_PAO_Effluent</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>1.870552976500988</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>X_PAO_Wastage</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>90.57472301947769</v>
+        <v>87.17321980105622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>